<commit_message>
change in xlsx config, delete unused config files
</commit_message>
<xml_diff>
--- a/nifi/application/config/xlsx_config/VO_ZA_CONFIG.xlsx
+++ b/nifi/application/config/xlsx_config/VO_ZA_CONFIG.xlsx
@@ -209,54 +209,7 @@
     <t xml:space="preserve">expect_column_values_to_be_in_set_2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">{'value_set' : ['pro','private','dealer','owner','professional',</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">particuliers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">], 'mostly' : 0.95}</t>
-    </r>
+    <t xml:space="preserve">{'value_set' : ['pro','private','dealer','owner','professional','particuliers'], 'mostly' : 0.95}</t>
   </si>
   <si>
     <t xml:space="preserve">VILLE</t>
@@ -314,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -357,12 +310,6 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -489,8 +436,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>